<commit_message>
update to the Product NEST and Warranty modules
</commit_message>
<xml_diff>
--- a/final.xlsx
+++ b/final.xlsx
@@ -853,64 +853,64 @@
     </border>
   </borders>
   <cellStyleXfs count="58">
-    <xf borderId="0" fillId="3" fontId="9" numFmtId="0"/>
+    <xf borderId="0" fillId="13" fontId="19" numFmtId="0"/>
+    <xf borderId="0" fillId="15" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
     <xf borderId="0" fillId="32" fontId="19" numFmtId="0"/>
-    <xf borderId="0" fillId="31" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="14" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="11" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="30" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="9" fontId="19" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0"/>
     <xf borderId="0" fillId="26" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="18" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="29" fontId="19" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0"/>
-    <xf borderId="0" fillId="11" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="5" fillId="6" fontId="12" numFmtId="0"/>
-    <xf borderId="0" fillId="21" fontId="19" numFmtId="0"/>
-    <xf borderId="0" fillId="25" fontId="19" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0"/>
-    <xf borderId="0" fillId="13" fontId="19" numFmtId="0"/>
-    <xf borderId="0" fillId="27" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="11" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="27" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="15" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="18" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="17" fontId="19" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="22" numFmtId="0"/>
-    <xf borderId="0" fillId="16" fontId="19" numFmtId="0"/>
-    <xf borderId="0" fillId="22" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0"/>
-    <xf borderId="0" fillId="15" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="30" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="14" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="9" fontId="19" numFmtId="0"/>
-    <xf borderId="8" fillId="8" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="28" fontId="19" numFmtId="0"/>
-    <xf borderId="3" fillId="0" fontId="7" numFmtId="0"/>
-    <xf borderId="0" fillId="23" fontId="3" numFmtId="0"/>
+    <xf borderId="4" fillId="6" fontId="13" numFmtId="0"/>
     <xf borderId="0" fillId="19" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="10" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="27" fontId="3" numFmtId="0"/>
+    <xf borderId="6" fillId="0" fontId="14" numFmtId="0"/>
+    <xf borderId="0" fillId="12" fontId="19" numFmtId="0"/>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0"/>
+    <xf borderId="0" fillId="17" fontId="19" numFmtId="0"/>
+    <xf borderId="0" fillId="22" fontId="3" numFmtId="0"/>
+    <xf borderId="4" fillId="5" fontId="11" numFmtId="0"/>
+    <xf borderId="0" fillId="18" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="14" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="20" fontId="19" numFmtId="0"/>
+    <xf borderId="0" fillId="24" fontId="19" numFmtId="0"/>
+    <xf borderId="0" fillId="26" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="22" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="28" fontId="19" numFmtId="0"/>
     <xf borderId="0" fillId="23" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="3" fillId="0" fontId="7" numFmtId="0"/>
+    <xf borderId="0" fillId="16" fontId="19" numFmtId="0"/>
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0"/>
+    <xf borderId="5" fillId="6" fontId="12" numFmtId="0"/>
+    <xf borderId="0" fillId="18" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="4" fontId="10" numFmtId="0"/>
+    <xf borderId="0" fillId="30" fontId="3" numFmtId="0"/>
+    <xf borderId="8" fillId="8" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="3" fontId="9" numFmtId="0"/>
+    <xf borderId="0" fillId="31" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="19" fontId="3" numFmtId="0"/>
+    <xf borderId="9" fillId="0" fontId="18" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="8" fillId="8" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="31" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="29" fontId="19" numFmtId="0"/>
+    <xf borderId="0" fillId="23" fontId="3" numFmtId="0"/>
+    <xf borderId="7" fillId="7" fontId="15" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="22" numFmtId="0"/>
     <xf borderId="2" fillId="0" fontId="6" numFmtId="0"/>
+    <xf borderId="0" fillId="14" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="22" numFmtId="0"/>
+    <xf borderId="0" fillId="25" fontId="19" numFmtId="0"/>
+    <xf borderId="0" fillId="21" fontId="19" numFmtId="0"/>
+    <xf borderId="0" fillId="27" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="10" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="24" fontId="19" numFmtId="0"/>
-    <xf borderId="4" fillId="5" fontId="11" numFmtId="0"/>
+    <xf borderId="0" fillId="11" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="15" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="17" numFmtId="0"/>
-    <xf borderId="4" fillId="6" fontId="13" numFmtId="0"/>
-    <xf borderId="0" fillId="30" fontId="3" numFmtId="0"/>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0"/>
-    <xf borderId="6" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
-    <xf borderId="9" fillId="0" fontId="18" numFmtId="0"/>
-    <xf borderId="0" fillId="22" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="31" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="12" fontId="19" numFmtId="0"/>
-    <xf borderId="8" fillId="8" fontId="3" numFmtId="0"/>
-    <xf borderId="7" fillId="7" fontId="15" numFmtId="0"/>
-    <xf borderId="0" fillId="26" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="22" numFmtId="0"/>
-    <xf borderId="0" fillId="20" fontId="19" numFmtId="0"/>
-    <xf borderId="0" fillId="4" fontId="10" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="56">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -1077,64 +1077,64 @@
     </xf>
   </cellXfs>
   <cellStyles count="58">
-    <cellStyle builtinId="27" name="Bad" xfId="0"/>
-    <cellStyle builtinId="52" name="60% - Accent6" xfId="1"/>
-    <cellStyle builtinId="51" name="40% - Accent6" xfId="2"/>
-    <cellStyle name="20% - Accent2 2" xfId="3"/>
-    <cellStyle builtinId="46" name="20% - Accent5" xfId="4"/>
-    <cellStyle name="20% - Accent3 2" xfId="5"/>
-    <cellStyle builtinId="49" name="Accent6" xfId="6"/>
-    <cellStyle builtinId="11" name="Warning Text" xfId="7"/>
-    <cellStyle name="40% - Accent1 2" xfId="8"/>
-    <cellStyle name="Normal 10" xfId="9"/>
-    <cellStyle builtinId="21" name="Output" xfId="10"/>
-    <cellStyle builtinId="41" name="Accent4" xfId="11"/>
-    <cellStyle builtinId="45" name="Accent5" xfId="12"/>
-    <cellStyle builtinId="19" name="Heading 4" xfId="13"/>
-    <cellStyle builtinId="33" name="Accent2" xfId="14"/>
-    <cellStyle builtinId="47" name="40% - Accent5" xfId="15"/>
-    <cellStyle builtinId="31" name="40% - Accent1" xfId="16"/>
-    <cellStyle name="40% - Accent5 2" xfId="17"/>
-    <cellStyle name="40% - Accent2 2" xfId="18"/>
-    <cellStyle builtinId="38" name="20% - Accent3" xfId="19"/>
-    <cellStyle builtinId="37" name="Accent3" xfId="20"/>
-    <cellStyle name="Percent 2" xfId="21"/>
-    <cellStyle builtinId="36" name="60% - Accent2" xfId="22"/>
-    <cellStyle name="20% - Accent4 2" xfId="23"/>
-    <cellStyle builtinId="26" name="Good" xfId="24"/>
-    <cellStyle builtinId="35" name="40% - Accent2" xfId="25"/>
-    <cellStyle builtinId="50" name="20% - Accent6" xfId="26"/>
-    <cellStyle builtinId="34" name="20% - Accent2" xfId="27"/>
-    <cellStyle builtinId="29" name="Accent1" xfId="28"/>
-    <cellStyle name="Note 2" xfId="29"/>
-    <cellStyle builtinId="48" name="60% - Accent5" xfId="30"/>
-    <cellStyle builtinId="18" name="Heading 3" xfId="31"/>
-    <cellStyle name="40% - Accent4 2" xfId="32"/>
-    <cellStyle builtinId="39" name="40% - Accent3" xfId="33"/>
-    <cellStyle builtinId="30" name="20% - Accent1" xfId="34"/>
-    <cellStyle builtinId="43" name="40% - Accent4" xfId="35"/>
-    <cellStyle name="Normal 9 2" xfId="36"/>
-    <cellStyle name="40% - Accent3 2" xfId="37"/>
-    <cellStyle builtinId="17" name="Heading 2" xfId="38"/>
-    <cellStyle name="20% - Accent1 2" xfId="39"/>
-    <cellStyle builtinId="44" name="60% - Accent4" xfId="40"/>
-    <cellStyle builtinId="20" name="Input" xfId="41"/>
-    <cellStyle builtinId="53" name="Explanatory Text" xfId="42"/>
-    <cellStyle builtinId="22" name="Calculation" xfId="43"/>
-    <cellStyle name="20% - Accent6 2" xfId="44"/>
-    <cellStyle builtinId="16" name="Heading 1" xfId="45"/>
-    <cellStyle builtinId="24" name="Linked Cell" xfId="46"/>
-    <cellStyle builtinId="15" name="Title" xfId="47"/>
-    <cellStyle builtinId="25" name="Total" xfId="48"/>
-    <cellStyle builtinId="42" name="20% - Accent4" xfId="49"/>
-    <cellStyle name="40% - Accent6 2" xfId="50"/>
-    <cellStyle builtinId="32" name="60% - Accent1" xfId="51"/>
-    <cellStyle builtinId="10" name="Note" xfId="52"/>
-    <cellStyle builtinId="23" name="Check Cell" xfId="53"/>
-    <cellStyle name="20% - Accent5 2" xfId="54"/>
-    <cellStyle builtinId="0" name="Normal" xfId="55"/>
-    <cellStyle builtinId="40" name="60% - Accent3" xfId="56"/>
-    <cellStyle builtinId="28" name="Neutral" xfId="57"/>
+    <cellStyle builtinId="33" name="Accent2" xfId="0"/>
+    <cellStyle builtinId="35" name="40% - Accent2" xfId="1"/>
+    <cellStyle builtinId="11" name="Warning Text" xfId="2"/>
+    <cellStyle builtinId="15" name="Title" xfId="3"/>
+    <cellStyle builtinId="52" name="60% - Accent6" xfId="4"/>
+    <cellStyle builtinId="31" name="40% - Accent1" xfId="5"/>
+    <cellStyle name="20% - Accent6 2" xfId="6"/>
+    <cellStyle builtinId="29" name="Accent1" xfId="7"/>
+    <cellStyle builtinId="19" name="Heading 4" xfId="8"/>
+    <cellStyle name="20% - Accent5 2" xfId="9"/>
+    <cellStyle builtinId="22" name="Calculation" xfId="10"/>
+    <cellStyle name="40% - Accent3 2" xfId="11"/>
+    <cellStyle builtinId="30" name="20% - Accent1" xfId="12"/>
+    <cellStyle builtinId="47" name="40% - Accent5" xfId="13"/>
+    <cellStyle builtinId="24" name="Linked Cell" xfId="14"/>
+    <cellStyle builtinId="32" name="60% - Accent1" xfId="15"/>
+    <cellStyle builtinId="16" name="Heading 1" xfId="16"/>
+    <cellStyle builtinId="37" name="Accent3" xfId="17"/>
+    <cellStyle name="20% - Accent4 2" xfId="18"/>
+    <cellStyle builtinId="20" name="Input" xfId="19"/>
+    <cellStyle builtinId="38" name="20% - Accent3" xfId="20"/>
+    <cellStyle builtinId="34" name="20% - Accent2" xfId="21"/>
+    <cellStyle builtinId="40" name="60% - Accent3" xfId="22"/>
+    <cellStyle builtinId="44" name="60% - Accent4" xfId="23"/>
+    <cellStyle builtinId="46" name="20% - Accent5" xfId="24"/>
+    <cellStyle builtinId="42" name="20% - Accent4" xfId="25"/>
+    <cellStyle builtinId="48" name="60% - Accent5" xfId="26"/>
+    <cellStyle name="40% - Accent4 2" xfId="27"/>
+    <cellStyle name="Normal 10" xfId="28"/>
+    <cellStyle builtinId="18" name="Heading 3" xfId="29"/>
+    <cellStyle builtinId="36" name="60% - Accent2" xfId="30"/>
+    <cellStyle builtinId="26" name="Good" xfId="31"/>
+    <cellStyle builtinId="21" name="Output" xfId="32"/>
+    <cellStyle name="20% - Accent3 2" xfId="33"/>
+    <cellStyle builtinId="28" name="Neutral" xfId="34"/>
+    <cellStyle builtinId="50" name="20% - Accent6" xfId="35"/>
+    <cellStyle builtinId="10" name="Note" xfId="36"/>
+    <cellStyle builtinId="27" name="Bad" xfId="37"/>
+    <cellStyle builtinId="51" name="40% - Accent6" xfId="38"/>
+    <cellStyle builtinId="39" name="40% - Accent3" xfId="39"/>
+    <cellStyle builtinId="25" name="Total" xfId="40"/>
+    <cellStyle name="Normal 9 2" xfId="41"/>
+    <cellStyle name="Note 2" xfId="42"/>
+    <cellStyle name="40% - Accent6 2" xfId="43"/>
+    <cellStyle builtinId="49" name="Accent6" xfId="44"/>
+    <cellStyle builtinId="43" name="40% - Accent4" xfId="45"/>
+    <cellStyle builtinId="23" name="Check Cell" xfId="46"/>
+    <cellStyle builtinId="0" name="Normal" xfId="47"/>
+    <cellStyle builtinId="17" name="Heading 2" xfId="48"/>
+    <cellStyle name="20% - Accent2 2" xfId="49"/>
+    <cellStyle name="Percent 2" xfId="50"/>
+    <cellStyle builtinId="45" name="Accent5" xfId="51"/>
+    <cellStyle builtinId="41" name="Accent4" xfId="52"/>
+    <cellStyle name="40% - Accent5 2" xfId="53"/>
+    <cellStyle name="20% - Accent1 2" xfId="54"/>
+    <cellStyle name="40% - Accent1 2" xfId="55"/>
+    <cellStyle name="40% - Accent2 2" xfId="56"/>
+    <cellStyle builtinId="53" name="Explanatory Text" xfId="57"/>
   </cellStyles>
   <dxfs count="12">
     <dxf>

</xml_diff>

<commit_message>
some code comments added
</commit_message>
<xml_diff>
--- a/final.xlsx
+++ b/final.xlsx
@@ -853,64 +853,64 @@
     </border>
   </borders>
   <cellStyleXfs count="58">
-    <xf borderId="0" fillId="13" fontId="19" numFmtId="0"/>
+    <xf borderId="0" fillId="21" fontId="19" numFmtId="0"/>
+    <xf borderId="0" fillId="27" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="31" fontId="3" numFmtId="0"/>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0"/>
+    <xf borderId="0" fillId="11" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="15" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="23" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="27" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="19" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="18" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="26" fontId="3" numFmtId="0"/>
+    <xf borderId="9" fillId="0" fontId="18" numFmtId="0"/>
+    <xf borderId="0" fillId="32" fontId="19" numFmtId="0"/>
+    <xf borderId="0" fillId="29" fontId="19" numFmtId="0"/>
+    <xf borderId="5" fillId="6" fontId="12" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="22" numFmtId="0"/>
+    <xf borderId="0" fillId="10" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="22" numFmtId="0"/>
+    <xf borderId="0" fillId="16" fontId="19" numFmtId="0"/>
+    <xf borderId="0" fillId="4" fontId="10" numFmtId="0"/>
+    <xf borderId="4" fillId="6" fontId="13" numFmtId="0"/>
+    <xf borderId="0" fillId="24" fontId="19" numFmtId="0"/>
+    <xf borderId="7" fillId="7" fontId="15" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="31" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="14" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="16" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
-    <xf borderId="0" fillId="32" fontId="19" numFmtId="0"/>
-    <xf borderId="0" fillId="11" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="30" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="9" fontId="19" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0"/>
-    <xf borderId="0" fillId="26" fontId="3" numFmtId="0"/>
-    <xf borderId="4" fillId="6" fontId="13" numFmtId="0"/>
-    <xf borderId="0" fillId="19" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="10" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="27" fontId="3" numFmtId="0"/>
-    <xf borderId="6" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="12" fontId="19" numFmtId="0"/>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0"/>
-    <xf borderId="0" fillId="17" fontId="19" numFmtId="0"/>
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0"/>
+    <xf borderId="0" fillId="25" fontId="19" numFmtId="0"/>
     <xf borderId="0" fillId="22" fontId="3" numFmtId="0"/>
-    <xf borderId="4" fillId="5" fontId="11" numFmtId="0"/>
-    <xf borderId="0" fillId="18" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="14" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="20" fontId="19" numFmtId="0"/>
-    <xf borderId="0" fillId="24" fontId="19" numFmtId="0"/>
-    <xf borderId="0" fillId="26" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="22" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="28" fontId="19" numFmtId="0"/>
     <xf borderId="0" fillId="23" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="3" fillId="0" fontId="7" numFmtId="0"/>
-    <xf borderId="0" fillId="16" fontId="19" numFmtId="0"/>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0"/>
-    <xf borderId="5" fillId="6" fontId="12" numFmtId="0"/>
-    <xf borderId="0" fillId="18" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="4" fontId="10" numFmtId="0"/>
-    <xf borderId="0" fillId="30" fontId="3" numFmtId="0"/>
-    <xf borderId="8" fillId="8" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="3" fontId="9" numFmtId="0"/>
-    <xf borderId="0" fillId="31" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="19" fontId="3" numFmtId="0"/>
-    <xf borderId="9" fillId="0" fontId="18" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="8" fillId="8" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="31" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="29" fontId="19" numFmtId="0"/>
-    <xf borderId="0" fillId="23" fontId="3" numFmtId="0"/>
-    <xf borderId="7" fillId="7" fontId="15" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="22" numFmtId="0"/>
     <xf borderId="2" fillId="0" fontId="6" numFmtId="0"/>
     <xf borderId="0" fillId="14" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="22" numFmtId="0"/>
-    <xf borderId="0" fillId="25" fontId="19" numFmtId="0"/>
-    <xf borderId="0" fillId="21" fontId="19" numFmtId="0"/>
-    <xf borderId="0" fillId="27" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="30" fontId="3" numFmtId="0"/>
+    <xf borderId="3" fillId="0" fontId="7" numFmtId="0"/>
+    <xf borderId="0" fillId="30" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="13" fontId="19" numFmtId="0"/>
+    <xf borderId="0" fillId="12" fontId="19" numFmtId="0"/>
+    <xf borderId="0" fillId="18" fontId="3" numFmtId="0"/>
+    <xf borderId="6" fillId="0" fontId="14" numFmtId="0"/>
+    <xf borderId="0" fillId="26" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="11" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="22" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="19" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="3" fontId="9" numFmtId="0"/>
+    <xf borderId="8" fillId="8" fontId="3" numFmtId="0"/>
+    <xf borderId="8" fillId="8" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="15" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="28" fontId="19" numFmtId="0"/>
+    <xf borderId="0" fillId="9" fontId="19" numFmtId="0"/>
+    <xf borderId="0" fillId="17" fontId="19" numFmtId="0"/>
+    <xf borderId="4" fillId="5" fontId="11" numFmtId="0"/>
     <xf borderId="0" fillId="10" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="11" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="15" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="56">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -1077,64 +1077,64 @@
     </xf>
   </cellXfs>
   <cellStyles count="58">
-    <cellStyle builtinId="33" name="Accent2" xfId="0"/>
-    <cellStyle builtinId="35" name="40% - Accent2" xfId="1"/>
-    <cellStyle builtinId="11" name="Warning Text" xfId="2"/>
-    <cellStyle builtinId="15" name="Title" xfId="3"/>
-    <cellStyle builtinId="52" name="60% - Accent6" xfId="4"/>
+    <cellStyle builtinId="41" name="Accent4" xfId="0"/>
+    <cellStyle builtinId="47" name="40% - Accent5" xfId="1"/>
+    <cellStyle builtinId="51" name="40% - Accent6" xfId="2"/>
+    <cellStyle builtinId="16" name="Heading 1" xfId="3"/>
+    <cellStyle builtinId="19" name="Heading 4" xfId="4"/>
     <cellStyle builtinId="31" name="40% - Accent1" xfId="5"/>
-    <cellStyle name="20% - Accent6 2" xfId="6"/>
-    <cellStyle builtinId="29" name="Accent1" xfId="7"/>
-    <cellStyle builtinId="19" name="Heading 4" xfId="8"/>
-    <cellStyle name="20% - Accent5 2" xfId="9"/>
-    <cellStyle builtinId="22" name="Calculation" xfId="10"/>
-    <cellStyle name="40% - Accent3 2" xfId="11"/>
-    <cellStyle builtinId="30" name="20% - Accent1" xfId="12"/>
-    <cellStyle builtinId="47" name="40% - Accent5" xfId="13"/>
-    <cellStyle builtinId="24" name="Linked Cell" xfId="14"/>
-    <cellStyle builtinId="32" name="60% - Accent1" xfId="15"/>
-    <cellStyle builtinId="16" name="Heading 1" xfId="16"/>
-    <cellStyle builtinId="37" name="Accent3" xfId="17"/>
-    <cellStyle name="20% - Accent4 2" xfId="18"/>
-    <cellStyle builtinId="20" name="Input" xfId="19"/>
-    <cellStyle builtinId="38" name="20% - Accent3" xfId="20"/>
-    <cellStyle builtinId="34" name="20% - Accent2" xfId="21"/>
-    <cellStyle builtinId="40" name="60% - Accent3" xfId="22"/>
-    <cellStyle builtinId="44" name="60% - Accent4" xfId="23"/>
-    <cellStyle builtinId="46" name="20% - Accent5" xfId="24"/>
-    <cellStyle builtinId="42" name="20% - Accent4" xfId="25"/>
-    <cellStyle builtinId="48" name="60% - Accent5" xfId="26"/>
-    <cellStyle name="40% - Accent4 2" xfId="27"/>
-    <cellStyle name="Normal 10" xfId="28"/>
-    <cellStyle builtinId="18" name="Heading 3" xfId="29"/>
-    <cellStyle builtinId="36" name="60% - Accent2" xfId="30"/>
-    <cellStyle builtinId="26" name="Good" xfId="31"/>
-    <cellStyle builtinId="21" name="Output" xfId="32"/>
-    <cellStyle name="20% - Accent3 2" xfId="33"/>
-    <cellStyle builtinId="28" name="Neutral" xfId="34"/>
-    <cellStyle builtinId="50" name="20% - Accent6" xfId="35"/>
-    <cellStyle builtinId="10" name="Note" xfId="36"/>
-    <cellStyle builtinId="27" name="Bad" xfId="37"/>
-    <cellStyle builtinId="51" name="40% - Accent6" xfId="38"/>
-    <cellStyle builtinId="39" name="40% - Accent3" xfId="39"/>
-    <cellStyle builtinId="25" name="Total" xfId="40"/>
-    <cellStyle name="Normal 9 2" xfId="41"/>
-    <cellStyle name="Note 2" xfId="42"/>
-    <cellStyle name="40% - Accent6 2" xfId="43"/>
-    <cellStyle builtinId="49" name="Accent6" xfId="44"/>
-    <cellStyle builtinId="43" name="40% - Accent4" xfId="45"/>
-    <cellStyle builtinId="23" name="Check Cell" xfId="46"/>
-    <cellStyle builtinId="0" name="Normal" xfId="47"/>
-    <cellStyle builtinId="17" name="Heading 2" xfId="48"/>
-    <cellStyle name="20% - Accent2 2" xfId="49"/>
-    <cellStyle name="Percent 2" xfId="50"/>
-    <cellStyle builtinId="45" name="Accent5" xfId="51"/>
-    <cellStyle builtinId="41" name="Accent4" xfId="52"/>
-    <cellStyle name="40% - Accent5 2" xfId="53"/>
-    <cellStyle name="20% - Accent1 2" xfId="54"/>
-    <cellStyle name="40% - Accent1 2" xfId="55"/>
-    <cellStyle name="40% - Accent2 2" xfId="56"/>
-    <cellStyle builtinId="53" name="Explanatory Text" xfId="57"/>
+    <cellStyle name="40% - Accent2 2" xfId="6"/>
+    <cellStyle name="40% - Accent4 2" xfId="7"/>
+    <cellStyle name="40% - Accent5 2" xfId="8"/>
+    <cellStyle builtinId="39" name="40% - Accent3" xfId="9"/>
+    <cellStyle builtinId="38" name="20% - Accent3" xfId="10"/>
+    <cellStyle name="20% - Accent5 2" xfId="11"/>
+    <cellStyle builtinId="25" name="Total" xfId="12"/>
+    <cellStyle builtinId="52" name="60% - Accent6" xfId="13"/>
+    <cellStyle builtinId="49" name="Accent6" xfId="14"/>
+    <cellStyle builtinId="21" name="Output" xfId="15"/>
+    <cellStyle builtinId="15" name="Title" xfId="16"/>
+    <cellStyle builtinId="0" name="Normal" xfId="17"/>
+    <cellStyle name="20% - Accent1 2" xfId="18"/>
+    <cellStyle builtinId="53" name="Explanatory Text" xfId="19"/>
+    <cellStyle name="Percent 2" xfId="20"/>
+    <cellStyle builtinId="36" name="60% - Accent2" xfId="21"/>
+    <cellStyle builtinId="28" name="Neutral" xfId="22"/>
+    <cellStyle builtinId="22" name="Calculation" xfId="23"/>
+    <cellStyle builtinId="44" name="60% - Accent4" xfId="24"/>
+    <cellStyle builtinId="23" name="Check Cell" xfId="25"/>
+    <cellStyle name="Normal 9 2" xfId="26"/>
+    <cellStyle name="40% - Accent6 2" xfId="27"/>
+    <cellStyle name="20% - Accent2 2" xfId="28"/>
+    <cellStyle builtinId="11" name="Warning Text" xfId="29"/>
+    <cellStyle builtinId="26" name="Good" xfId="30"/>
+    <cellStyle builtinId="45" name="Accent5" xfId="31"/>
+    <cellStyle builtinId="42" name="20% - Accent4" xfId="32"/>
+    <cellStyle builtinId="40" name="60% - Accent3" xfId="33"/>
+    <cellStyle builtinId="43" name="40% - Accent4" xfId="34"/>
+    <cellStyle builtinId="17" name="Heading 2" xfId="35"/>
+    <cellStyle builtinId="34" name="20% - Accent2" xfId="36"/>
+    <cellStyle name="20% - Accent6 2" xfId="37"/>
+    <cellStyle builtinId="18" name="Heading 3" xfId="38"/>
+    <cellStyle builtinId="50" name="20% - Accent6" xfId="39"/>
+    <cellStyle builtinId="33" name="Accent2" xfId="40"/>
+    <cellStyle builtinId="32" name="60% - Accent1" xfId="41"/>
+    <cellStyle name="20% - Accent3 2" xfId="42"/>
+    <cellStyle builtinId="24" name="Linked Cell" xfId="43"/>
+    <cellStyle builtinId="46" name="20% - Accent5" xfId="44"/>
+    <cellStyle name="40% - Accent1 2" xfId="45"/>
+    <cellStyle name="20% - Accent4 2" xfId="46"/>
+    <cellStyle name="40% - Accent3 2" xfId="47"/>
+    <cellStyle builtinId="27" name="Bad" xfId="48"/>
+    <cellStyle name="Note 2" xfId="49"/>
+    <cellStyle builtinId="10" name="Note" xfId="50"/>
+    <cellStyle name="Normal 10" xfId="51"/>
+    <cellStyle builtinId="35" name="40% - Accent2" xfId="52"/>
+    <cellStyle builtinId="48" name="60% - Accent5" xfId="53"/>
+    <cellStyle builtinId="29" name="Accent1" xfId="54"/>
+    <cellStyle builtinId="37" name="Accent3" xfId="55"/>
+    <cellStyle builtinId="20" name="Input" xfId="56"/>
+    <cellStyle builtinId="30" name="20% - Accent1" xfId="57"/>
   </cellStyles>
   <dxfs count="12">
     <dxf>

</xml_diff>